<commit_message>
changed test to compile
</commit_message>
<xml_diff>
--- a/src/test/resources/Executables/book1.xlsx
+++ b/src/test/resources/Executables/book1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2809" uniqueCount="198">
   <si>
     <t>FilePaths</t>
   </si>
@@ -596,6 +596,30 @@
   </si>
   <si>
     <t>EMIs from ₹11,124/month</t>
+  </si>
+  <si>
+    <t>₹5.14 Lakh</t>
+  </si>
+  <si>
+    <t>EMIs from ₹10,044/month</t>
+  </si>
+  <si>
+    <t>₹8.70 Lakh</t>
+  </si>
+  <si>
+    <t>EMIs from ₹16,560/month</t>
+  </si>
+  <si>
+    <t>2017 Maruti Swift ZXI</t>
+  </si>
+  <si>
+    <t>63,367 KM</t>
+  </si>
+  <si>
+    <t>₹5.43 Lakh</t>
+  </si>
+  <si>
+    <t>EMIs from ₹10,616/month</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1031,10 @@
         <v>37</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2">
@@ -1041,22 +1065,22 @@
         <v>5</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>174</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>175</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>177</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
@@ -1087,22 +1111,22 @@
         <v>7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>178</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>179</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>98</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
@@ -1110,22 +1134,22 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
@@ -1133,22 +1157,22 @@
         <v>9</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>169</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -1156,22 +1180,22 @@
         <v>10</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>137</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9">
@@ -1179,22 +1203,22 @@
         <v>11</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>94</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -1202,22 +1226,22 @@
         <v>12</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>69</v>
+        <v>184</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>70</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11">
@@ -1225,22 +1249,22 @@
         <v>13</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>165</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12">
@@ -1248,22 +1272,22 @@
         <v>14</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13">
@@ -1294,10 +1318,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>29</v>
@@ -1306,10 +1330,10 @@
         <v>51</v>
       </c>
       <c r="F14" t="s" s="0">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15">
@@ -1317,22 +1341,22 @@
         <v>17</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>39</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16">
@@ -1340,22 +1364,22 @@
         <v>18</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>184</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>185</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
@@ -1363,22 +1387,22 @@
         <v>19</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="D17" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>105</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18">
@@ -1386,22 +1410,22 @@
         <v>20</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -1409,22 +1433,22 @@
         <v>21</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s" s="0">
         <v>29</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20">
@@ -1432,22 +1456,22 @@
         <v>22</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in xpath as per site updation
</commit_message>
<xml_diff>
--- a/src/test/resources/Executables/book1.xlsx
+++ b/src/test/resources/Executables/book1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumHcodeFramework\src\test\resources\Executables\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="126">
   <si>
     <t>FilePaths</t>
   </si>
@@ -359,12 +359,58 @@
   </si>
   <si>
     <t>/src/test/resources/Executables/download.jpg</t>
+  </si>
+  <si>
+    <t>2017 Maruti Baleno SIGMA PETROL 1.2</t>
+  </si>
+  <si>
+    <t>17,350 KM</t>
+  </si>
+  <si>
+    <t>₹4.98 Lakh</t>
+  </si>
+  <si>
+    <t>EMIs from ₹9,736/month</t>
+  </si>
+  <si>
+    <t>2018 Maruti Wagon R 1.0 LXI CNG</t>
+  </si>
+  <si>
+    <t>41,438 KM</t>
+  </si>
+  <si>
+    <t>₹4.05 Lakh</t>
+  </si>
+  <si>
+    <t>EMIs from ₹7,918/month</t>
+  </si>
+  <si>
+    <t>2020 Maruti Ciaz DELTA AT 1.5 SHVS PETROL</t>
+  </si>
+  <si>
+    <t>57,803 KM</t>
+  </si>
+  <si>
+    <t>₹7.89 Lakh</t>
+  </si>
+  <si>
+    <t>EMIs from ₹15,425/month</t>
+  </si>
+  <si>
+    <t>61,569 KM</t>
+  </si>
+  <si>
+    <t>₹1.60 Lakh</t>
+  </si>
+  <si>
+    <t>EMIs from ₹14,216/month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -733,12 +779,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>110</v>
       </c>
     </row>
@@ -758,463 +804,463 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F4" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G4" t="s" s="0">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F6" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G6" t="s" s="0">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F9" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E12" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F19" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="F20" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G20" t="s" s="0">
         <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>